<commit_message>
Seeding script is working from npm run db:setup script in package.json.
</commit_message>
<xml_diff>
--- a/utils/movies.xlsx
+++ b/utils/movies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fec\db work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fec\betacritic\bill-morelike-component\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA5A4AB-8E69-4E07-BB37-B3AF23F912C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151D2F33-C9FA-45CB-BDC3-808CC44087F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF11567A-78C4-44C9-96C1-C21AFE741701}"/>
   </bookViews>
@@ -949,7 +949,7 @@
     <t>North by Northwest</t>
   </si>
   <si>
-    <t>Yankee Doodle Dandy</t>
+    <t>Yankee Doodle Doodly Doo</t>
   </si>
 </sst>
 </file>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>304</v>

</xml_diff>

<commit_message>
Small update to movies source file.
</commit_message>
<xml_diff>
--- a/utils/movies.xlsx
+++ b/utils/movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fec\betacritic\bill-morelike-component\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151D2F33-C9FA-45CB-BDC3-808CC44087F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D53931-5526-42CE-8AF7-745F93137FF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF11567A-78C4-44C9-96C1-C21AFE741701}"/>
   </bookViews>
@@ -949,7 +949,7 @@
     <t>North by Northwest</t>
   </si>
   <si>
-    <t>Yankee Doodle Doodly Doo</t>
+    <t>Yankee Doodle Dandy</t>
   </si>
 </sst>
 </file>

</xml_diff>